<commit_message>
tested distance from OSM
</commit_message>
<xml_diff>
--- a/FE/commData.xlsx
+++ b/FE/commData.xlsx
@@ -483,12 +483,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>14.7661</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>120.9342</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>14.7661</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -521,12 +521,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>14.7653</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>120.9437</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>14.7653</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -559,12 +559,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>14.7535</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>120.9533</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>14.7535</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -597,12 +597,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>14.7738</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>120.9785</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>14.7738</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -635,12 +635,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>14.7603</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>120.9623</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>14.7603</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -677,12 +677,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>14.7911</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>121.0077</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>14.7911</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -715,12 +715,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>14.7465</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>120.941</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>14.7465</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -753,12 +753,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>14.7774</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>120.9595</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>14.7774</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -791,12 +791,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>14.7559</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>120.9488</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>14.7559</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -829,12 +829,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>14.7599</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>120.9464</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>14.7599</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -867,12 +867,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>14.7833</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>120.9849</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>14.7833</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -905,12 +905,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>14.7813</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>120.9868</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>14.7813</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -943,12 +943,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>14.7789</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>120.9746</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>14.7789</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -981,12 +981,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>14.784</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>120.9686</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>14.784</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1019,12 +1019,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>14.7642</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>120.9556</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>14.7642</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1057,12 +1057,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>14.7649</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>120.9488</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>14.7649</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">

</xml_diff>

<commit_message>
pathfinding, BNT, map update, display of data, solving progress
TODO: cancel btn, community/shelter slider, loading bar.
</commit_message>
<xml_diff>
--- a/FE/commData.xlsx
+++ b/FE/commData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>VulPop</t>
+          <t>AffectedPop</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -465,6 +465,11 @@
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MaxDistance</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
@@ -473,39 +478,614 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DummyName</t>
+          <t>Abangan Norte</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>14.7661</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>120.9342</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>11417</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>10080</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>6431</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Sample remarks</t>
-        </is>
-      </c>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Abangan Sur</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>14.7653</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>120.9437</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10595</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>9750</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>6525</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ibayo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>14.7535</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>120.9533</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8310</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>7186</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Lambakin</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>14.7738</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>120.9785</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>48184</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>30000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>27645</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Lias</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>14.7603</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>120.9623</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>15256</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1545</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>8801</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>hmmm yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Loma de Gato</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>14.7911</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>121.0077</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>71258</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>38463</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Nagbalon</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>14.7465</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>120.941</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3518</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4925</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2829</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Patubig</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>14.7774</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>120.9595</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>8419</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>5343</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Poblacion I</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>14.7559</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>120.9488</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1419</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1212</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Poblacion II</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>14.7599</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>120.9464</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4968</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>3918</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Prenza I</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14.7833</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>120.9849</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>9019</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>4705</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Prenza II</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14.7813</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>120.9868</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>13784</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3050</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>7475</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Santa Rosa I</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>14.7789</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>120.9746</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>11260</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>4995</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>7268</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Santa Rosa II</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>14.784</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>120.9686</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>13378</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>4500</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>6385</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Saog</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>14.7642</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>120.9556</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>15612</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>10458</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Tabing Ilog</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>14.7649</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>120.9488</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>8056</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>5500</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>4989</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>